<commit_message>
Added timing error to tof model
</commit_message>
<xml_diff>
--- a/model/System Model.xlsx
+++ b/model/System Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\IIB Project\System Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\IIB Project\iib-project\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF649F7A-FAA4-4AA2-9E89-65B8F94B9B07}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D27BFD8-D0CB-400F-98F1-90D0E582987D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{2E20499A-CF7D-441A-9B23-3C755E67DBA1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{2E20499A-CF7D-441A-9B23-3C755E67DBA1}"/>
   </bookViews>
   <sheets>
     <sheet name="System Blocks" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
   <si>
     <t>TX Power (dBm)</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>Required Link Margin (dB)</t>
-  </si>
-  <si>
-    <t>Noise Budget</t>
   </si>
   <si>
     <t>Antenna Noise Temperature (K)</t>
@@ -516,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -559,15 +556,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -650,38 +638,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1650,18 +1644,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
     </row>
     <row r="3" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1677,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C58272F-101F-4B99-AF78-72AA6E441E3F}">
   <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,22 +1681,22 @@
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="4" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="30.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="40"/>
+    <col min="8" max="8" width="12" style="37" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="37"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="G2" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="29"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="G2" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="62"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15"/>
@@ -1722,10 +1716,10 @@
       <c r="G4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="35" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1740,12 +1734,12 @@
         <v>100</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="33">
+        <v>20</v>
+      </c>
+      <c r="H5" s="30">
         <v>290</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="27">
         <v>290</v>
       </c>
     </row>
@@ -1761,14 +1755,14 @@
         <f>10*LOG(D5,10)</f>
         <v>20</v>
       </c>
-      <c r="G6" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="34">
+      <c r="G6" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="31">
         <f>10*LOG(1.38E-23*1000*15360000*H5)</f>
         <v>-102.11331700004314</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="28">
         <f>10*LOG(1.38E-23*1000*15360000*I5)</f>
         <v>-102.11331700004314</v>
       </c>
@@ -1783,14 +1777,14 @@
       <c r="D7" s="6">
         <v>6</v>
       </c>
-      <c r="G7" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="45">
+      <c r="G7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="42">
         <f>C16</f>
         <v>-61.046224834232135</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="28">
         <f>D16</f>
         <v>-90.588649928625387</v>
       </c>
@@ -1805,14 +1799,14 @@
       <c r="D8" s="7">
         <v>3</v>
       </c>
-      <c r="G8" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="36">
+      <c r="G8" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="33">
         <f>H7-H6</f>
         <v>41.067092165811005</v>
       </c>
-      <c r="I8" s="41">
+      <c r="I8" s="38">
         <f>I7-I6</f>
         <v>11.524667071417753</v>
       </c>
@@ -1822,8 +1816,8 @@
       <c r="C9" s="13"/>
       <c r="D9" s="6"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="29"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -1836,12 +1830,12 @@
         <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="33">
+        <v>23</v>
+      </c>
+      <c r="H10" s="30">
         <v>0</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="27">
         <v>0</v>
       </c>
     </row>
@@ -1856,12 +1850,12 @@
         <v>2400</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="35">
+        <v>24</v>
+      </c>
+      <c r="H11" s="32">
         <v>2.62</v>
       </c>
-      <c r="I11" s="32">
+      <c r="I11" s="29">
         <v>2.62</v>
       </c>
     </row>
@@ -1869,21 +1863,21 @@
       <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="22">
         <f>20*LOG10(C10*1000)+20*LOG10(C11*1000000)-147.558</f>
         <v>100.04622483423213</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="21">
         <f>20*LOG10(D10*1000)+20*LOG10(D11*1000000)-147.558</f>
         <v>129.58864992862539</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="35">
+        <v>25</v>
+      </c>
+      <c r="H12" s="32">
         <v>3.5</v>
       </c>
-      <c r="I12" s="32">
+      <c r="I12" s="29">
         <v>3.5</v>
       </c>
     </row>
@@ -1897,14 +1891,14 @@
       <c r="D13" s="7">
         <v>0</v>
       </c>
-      <c r="G13" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="42">
+      <c r="G13" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="39">
         <f>H8-H10-H11-H12</f>
         <v>34.947092165811007</v>
       </c>
-      <c r="I13" s="41">
+      <c r="I13" s="38">
         <f>I8-I11-I12</f>
         <v>5.4046670714177516</v>
       </c>
@@ -1926,14 +1920,14 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="43">
+      <c r="B16" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="40">
         <f>C6+C7-C8-C12+C15</f>
         <v>-61.046224834232135</v>
       </c>
-      <c r="D16" s="44">
+      <c r="D16" s="41">
         <f>D6+D7-D8-D12+D15</f>
         <v>-90.588649928625387</v>
       </c>
@@ -1980,11 +1974,11 @@
       <c r="B21" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C21" s="20">
         <f>C16-C18+C19-C20</f>
         <v>-42.646224834232136</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="23">
         <f>D16-D18+D19-D20</f>
         <v>-72.188649928625381</v>
       </c>
@@ -2009,11 +2003,11 @@
       <c r="B24" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="20">
         <f>C21-C23</f>
         <v>-45.646224834232136</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="23">
         <f>D21-D23</f>
         <v>-75.188649928625381</v>
       </c>
@@ -2032,7 +2026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58112840-0D4D-4BF1-B983-15FAC19D934D}">
   <dimension ref="B3:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
@@ -2047,83 +2041,83 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="H3" s="53" t="s">
+      <c r="B3" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="H3" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="N3" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="N3" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="62"/>
     </row>
     <row r="4" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H4" s="15"/>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
-      <c r="K4" s="46"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
+      <c r="K4" s="43"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
     </row>
     <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="48" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="51" t="s">
-        <v>34</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="47" t="s">
+      <c r="K5" s="45" t="s">
         <v>31</v>
-      </c>
-      <c r="K5" s="48" t="s">
-        <v>32</v>
       </c>
       <c r="N5" s="16" t="s">
         <v>8</v>
       </c>
       <c r="O5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="47" t="s">
+      <c r="Q5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="Q5" s="48" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="54" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="55">
+      <c r="B6" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="51">
         <v>25.617000000000001</v>
       </c>
-      <c r="D6" s="58">
+      <c r="D6" s="54">
         <f>I22</f>
         <v>-70.816790199756866</v>
       </c>
-      <c r="E6" s="61">
+      <c r="E6" s="57">
         <f>O14</f>
         <v>6.7765268002862662</v>
       </c>
@@ -2140,30 +2134,30 @@
         <v>100</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O6" s="33">
+        <v>20</v>
+      </c>
+      <c r="O6" s="30">
         <v>290</v>
       </c>
-      <c r="P6" s="33">
+      <c r="P6" s="30">
         <v>290</v>
       </c>
-      <c r="Q6" s="30">
+      <c r="Q6" s="27">
         <v>290</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="57">
+      <c r="B7" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="53">
         <v>25.831</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="55">
         <f>J22</f>
         <v>-70.889049222565149</v>
       </c>
-      <c r="E7" s="62">
+      <c r="E7" s="58">
         <f>P14</f>
         <v>6.704267777477984</v>
       </c>
@@ -2182,34 +2176,34 @@
         <f>10*LOG(K6,10)</f>
         <v>20</v>
       </c>
-      <c r="N7" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" s="34">
+      <c r="N7" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="31">
         <f>10*LOG(1.38E-23*1000*15360000*O6)</f>
         <v>-102.11331700004314</v>
       </c>
-      <c r="P7" s="34">
+      <c r="P7" s="31">
         <f>10*LOG(1.38E-23*1000*15360000*P6)</f>
         <v>-102.11331700004314</v>
       </c>
-      <c r="Q7" s="31">
+      <c r="Q7" s="28">
         <f>10*LOG(1.38E-23*1000*15360000*Q6)</f>
         <v>-102.11331700004314</v>
       </c>
     </row>
     <row r="8" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="49" t="s">
-        <v>32</v>
+      <c r="B8" s="46" t="s">
+        <v>31</v>
       </c>
       <c r="C8" s="14">
         <v>25.597000000000001</v>
       </c>
-      <c r="D8" s="60">
+      <c r="D8" s="56">
         <f>K22</f>
         <v>-70.810006203131223</v>
       </c>
-      <c r="E8" s="63">
+      <c r="E8" s="59">
         <f>Q14</f>
         <v>6.7833107969119091</v>
       </c>
@@ -2225,18 +2219,18 @@
       <c r="K8" s="6">
         <v>6</v>
       </c>
-      <c r="N8" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8" s="45">
+      <c r="N8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" s="42">
         <f>I17</f>
         <v>-89.216790199756872</v>
       </c>
-      <c r="P8" s="34">
+      <c r="P8" s="31">
         <f>J17</f>
         <v>-89.289049222565154</v>
       </c>
-      <c r="Q8" s="31">
+      <c r="Q8" s="28">
         <f>K17</f>
         <v>-89.210006203131229</v>
       </c>
@@ -2254,18 +2248,18 @@
       <c r="K9" s="7">
         <v>3</v>
       </c>
-      <c r="N9" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="O9" s="36">
+      <c r="N9" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="33">
         <f>O8-O7</f>
         <v>12.896526800286267</v>
       </c>
-      <c r="P9" s="42">
+      <c r="P9" s="39">
         <f>P8-P7</f>
         <v>12.824267777477985</v>
       </c>
-      <c r="Q9" s="41">
+      <c r="Q9" s="38">
         <f>Q8-Q7</f>
         <v>12.90331079691191</v>
       </c>
@@ -2276,9 +2270,9 @@
       <c r="J10" s="13"/>
       <c r="K10" s="6"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="29"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H11" s="1" t="s">
@@ -2297,15 +2291,15 @@
         <v>25.597000000000001</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O11" s="33">
+        <v>23</v>
+      </c>
+      <c r="O11" s="30">
         <v>0</v>
       </c>
-      <c r="P11" s="33">
+      <c r="P11" s="30">
         <v>0</v>
       </c>
-      <c r="Q11" s="30">
+      <c r="Q11" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2323,15 +2317,15 @@
         <v>2400</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O12" s="35">
+        <v>24</v>
+      </c>
+      <c r="O12" s="32">
         <v>2.62</v>
       </c>
-      <c r="P12" s="35">
+      <c r="P12" s="32">
         <v>2.62</v>
       </c>
-      <c r="Q12" s="32">
+      <c r="Q12" s="29">
         <v>2.62</v>
       </c>
     </row>
@@ -2339,28 +2333,28 @@
       <c r="H13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="22">
         <f>20*LOG10(I11*1000)+20*LOG10(I12*1000000)-147.558</f>
         <v>128.21679019975687</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13" s="22">
         <f>20*LOG10(J11*1000)+20*LOG10(J12*1000000)-147.558</f>
         <v>128.28904922256515</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="21">
         <f>20*LOG10(K11*1000)+20*LOG10(K12*1000000)-147.558</f>
         <v>128.21000620313123</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O13" s="35">
+        <v>25</v>
+      </c>
+      <c r="O13" s="32">
         <v>3.5</v>
       </c>
-      <c r="P13" s="35">
+      <c r="P13" s="32">
         <v>3.5</v>
       </c>
-      <c r="Q13" s="32">
+      <c r="Q13" s="29">
         <v>3.5</v>
       </c>
     </row>
@@ -2377,18 +2371,18 @@
       <c r="K14" s="7">
         <v>0</v>
       </c>
-      <c r="N14" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="42">
+      <c r="N14" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="O14" s="39">
         <f>O9-O11-O12-O13</f>
         <v>6.7765268002862662</v>
       </c>
-      <c r="P14" s="42">
+      <c r="P14" s="39">
         <f>P9-P12-P13</f>
         <v>6.704267777477984</v>
       </c>
-      <c r="Q14" s="41">
+      <c r="Q14" s="38">
         <f>Q9-Q12-Q13</f>
         <v>6.7833107969119091</v>
       </c>
@@ -2398,9 +2392,9 @@
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
       <c r="K15" s="6"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H16" s="1" t="s">
@@ -2415,35 +2409,35 @@
       <c r="K16" s="5">
         <v>16</v>
       </c>
-      <c r="O16" s="40"/>
-      <c r="P16" s="40"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
     </row>
     <row r="17" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H17" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="43">
+      <c r="H17" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="40">
         <f>I7+I8-I9-I13+I16</f>
         <v>-89.216790199756872</v>
       </c>
-      <c r="J17" s="43">
+      <c r="J17" s="40">
         <f>J7+J8-J9-J13+J16</f>
         <v>-89.289049222565154</v>
       </c>
-      <c r="K17" s="44">
+      <c r="K17" s="41">
         <f>K7+K8-K9-K13+K16</f>
         <v>-89.210006203131229</v>
       </c>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
     </row>
     <row r="18" spans="8:16" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H18" s="2"/>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="K18" s="6"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
     </row>
     <row r="19" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H19" s="1" t="s">
@@ -2458,8 +2452,8 @@
       <c r="K19" s="5">
         <v>1.6</v>
       </c>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
     </row>
     <row r="20" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H20" s="2" t="s">
@@ -2474,8 +2468,8 @@
       <c r="K20" s="6">
         <v>23</v>
       </c>
-      <c r="O20" s="40"/>
-      <c r="P20" s="40"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
     </row>
     <row r="21" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H21" s="2" t="s">
@@ -2490,35 +2484,35 @@
       <c r="K21" s="6">
         <v>3</v>
       </c>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
     </row>
     <row r="22" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H22" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I22" s="23">
+      <c r="I22" s="20">
         <f>I17-I19+I20-I21</f>
         <v>-70.816790199756866</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J22" s="20">
         <f>J17-J19+J20-J21</f>
         <v>-70.889049222565149</v>
       </c>
-      <c r="K22" s="26">
+      <c r="K22" s="23">
         <f>K17-K19+K20-K21</f>
         <v>-70.810006203131223</v>
       </c>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
     </row>
     <row r="23" spans="8:16" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H23" s="3"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
       <c r="K23" s="6"/>
-      <c r="O23" s="40"/>
-      <c r="P23" s="40"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="37"/>
     </row>
     <row r="24" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H24" s="1" t="s">
@@ -2533,43 +2527,43 @@
       <c r="K24" s="5">
         <v>3</v>
       </c>
-      <c r="O24" s="40"/>
-      <c r="P24" s="40"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
     </row>
     <row r="25" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H25" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="23">
+      <c r="I25" s="20">
         <f>I22-I24</f>
         <v>-73.816790199756866</v>
       </c>
-      <c r="J25" s="23">
+      <c r="J25" s="20">
         <f>J22-J24</f>
         <v>-73.889049222565149</v>
       </c>
-      <c r="K25" s="26">
+      <c r="K25" s="23">
         <f>K22-K24</f>
         <v>-73.810006203131223</v>
       </c>
-      <c r="O25" s="40"/>
-      <c r="P25" s="40"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
     </row>
     <row r="26" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="O26" s="40"/>
-      <c r="P26" s="40"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
     </row>
     <row r="27" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="O27" s="40"/>
-      <c r="P27" s="40"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
     </row>
     <row r="28" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="O28" s="40"/>
-      <c r="P28" s="40"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="37"/>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>